<commit_message>
fix on nullable field reader
</commit_message>
<xml_diff>
--- a/AutoOpenXmlTest/Resources/input.xlsx
+++ b/AutoOpenXmlTest/Resources/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ruan.fachini\source\repos\ObjectToExcelFile\AutoOpenXmlTest\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\projets - Pessoais\AutoOpenXML\AutoOpenXmlTest\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{914E9598-12EA-418F-B1B8-D9922D3AC0B8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69E293D-950F-4865-AF18-723C58FD3B19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Nome</t>
   </si>
@@ -40,14 +40,23 @@
   </si>
   <si>
     <t>Ruan</t>
+  </si>
+  <si>
+    <t>Fabricio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -73,11 +82,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -406,7 +417,7 @@
     <col min="4" max="4" width="11.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,8 +431,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
@@ -433,10 +444,21 @@
       <c r="D2" s="3">
         <v>33478</v>
       </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F13" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Página &amp;P</oddFooter>

</xml_diff>

<commit_message>
Update on test Cases
</commit_message>
<xml_diff>
--- a/AutoOpenXmlTest/Resources/input.xlsx
+++ b/AutoOpenXmlTest/Resources/input.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\projets - Pessoais\AutoOpenXML\AutoOpenXmlTest\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CF7CD9E-FCF2-4316-BD19-6F034A1FFDB5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB109A3-8321-49C3-9C69-101A293E0DF4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="2" r:id="rId1"/>
+    <sheet name="DateTimeProperty" sheetId="5" r:id="rId1"/>
+    <sheet name="DateTimeNullableProperty" sheetId="4" r:id="rId2"/>
+    <sheet name="BoolNullableProperty" sheetId="2" r:id="rId3"/>
+    <sheet name="BoolProperty" sheetId="3" r:id="rId4"/>
+    <sheet name="DecimalNullableProperty" sheetId="6" r:id="rId5"/>
+    <sheet name="DecimalProperty" sheetId="7" r:id="rId6"/>
+    <sheet name="ModelIntNullableProperty" sheetId="8" r:id="rId7"/>
+    <sheet name="IntProperty" sheetId="9" r:id="rId8"/>
+    <sheet name="StringProperty" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="7">
   <si>
     <t>Ativo</t>
   </si>
@@ -87,7 +95,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -95,6 +103,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,11 +405,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B627EF7-54F6-4DAF-8983-5EB300419823}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -458,4 +467,524 @@
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668D0D30-24DA-4C11-9B96-AC2F8A17B9EC}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
+        <v>12233.45</v>
+      </c>
+      <c r="C2" s="4">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5">
+        <v>33478</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
+        <v>12233.45</v>
+      </c>
+      <c r="C2" s="4">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5">
+        <v>33478</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45A3162F-E2D0-4DEE-95DF-B81FDF5B8A81}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
+        <v>12233.45</v>
+      </c>
+      <c r="C2" s="4">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5">
+        <v>33478</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A4B40F5-D1AE-4B57-8726-83CBF1734B94}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
+        <v>12233.45</v>
+      </c>
+      <c r="C2" s="4">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5">
+        <v>33478</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2865B504-4FB8-42F9-9B12-D5425DCB9606}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
+        <v>12233.45</v>
+      </c>
+      <c r="C2" s="4">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5">
+        <v>33478</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B484994A-3F91-426E-92A4-9D525C7C30EF}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
+        <v>12233.45</v>
+      </c>
+      <c r="C2" s="4">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5">
+        <v>33478</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D62167-30BA-4903-AA5C-D598EDDFE1F2}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
+        <v>12233.45</v>
+      </c>
+      <c r="C2" s="4">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5">
+        <v>33478</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8459388-3215-41C8-8DC7-8291FC56FEC2}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
+        <v>12233.45</v>
+      </c>
+      <c r="C2" s="4">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5">
+        <v>33478</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3">
+        <v>123</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed bug, read formula cell
</commit_message>
<xml_diff>
--- a/AutoOpenXmlTest/Resources/input.xlsx
+++ b/AutoOpenXmlTest/Resources/input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\projets - Pessoais\AutoOpenXML\AutoOpenXmlTest\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mauricio.andre\source\private\AutoOpenXML\AutoOpenXmlTest\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A826A82F-3E6A-4DA9-AE18-4B2BA5F26106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93605C09-E412-4E40-BD05-F26B5D517BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="909" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="909" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DateTimeProperty" sheetId="5" r:id="rId1"/>
@@ -21,14 +21,27 @@
     <sheet name="DecimalProperty" sheetId="7" r:id="rId6"/>
     <sheet name="ModelIntNullableProperty" sheetId="8" r:id="rId7"/>
     <sheet name="IntProperty" sheetId="9" r:id="rId8"/>
-    <sheet name="StringProperty" sheetId="10" r:id="rId9"/>
+    <sheet name="FormulaProperty" sheetId="11" r:id="rId9"/>
+    <sheet name="StringProperty" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="10">
   <si>
     <t>Ativo</t>
   </si>
@@ -49,6 +62,15 @@
   </si>
   <si>
     <t>Fabricio</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Valor1</t>
+  </si>
+  <si>
+    <t>Valor2</t>
   </si>
 </sst>
 </file>
@@ -472,6 +494,71 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8459388-3215-41C8-8DC7-8291FC56FEC2}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3">
+        <v>12233.45</v>
+      </c>
+      <c r="C2" s="4">
+        <v>18</v>
+      </c>
+      <c r="D2" s="5">
+        <v>33478</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3">
+        <v>123</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{668D0D30-24DA-4C11-9B96-AC2F8A17B9EC}">
   <dimension ref="A1:I10"/>
@@ -871,7 +958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48D62167-30BA-4903-AA5C-D598EDDFE1F2}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -935,66 +1022,57 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8459388-3215-41C8-8DC7-8291FC56FEC2}">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE8696C-C43D-4A35-906A-9249D135271D}">
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>2+3</f>
+        <v>5</v>
+      </c>
+      <c r="F2">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="5" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>2*4</f>
+        <v>8</v>
+      </c>
+      <c r="G3">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3">
-        <v>12233.45</v>
-      </c>
-      <c r="C2" s="4">
-        <v>18</v>
-      </c>
-      <c r="D2" s="5">
-        <v>33478</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3">
-        <v>123</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I10" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>SUM(A2:A3)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>F2+G3</f>
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>